<commit_message>
Update Digital Marketing Plan.xlsx
</commit_message>
<xml_diff>
--- a/wp/documents/digital marketing plan/Digital Marketing Plan.xlsx
+++ b/wp/documents/digital marketing plan/Digital Marketing Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1-MyData\4-Projects\28-WebPicker\WebPicker-Local\wp\documents\digital marketing plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1-MyData\4-Projects\28-WebPicker\WebPicker-Github\webpicker\wp\documents\digital marketing plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A28938-D6C7-40FA-867C-233C7272DE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09428E7C-366A-4FA2-94DC-54ABCC0D22DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="130">
   <si>
     <t>WebPicker - Digital Marketing Plan &amp; Pricing Model</t>
   </si>
@@ -638,6 +638,16 @@
   <si>
     <t>https://developers.google.com/search/docs/advanced/robots/create-robots-txt?visit_id=637598707007128202-2171794991&amp;rd=1
 https://support.google.com/webmasters/answer/6062598</t>
+  </si>
+  <si>
+    <t>Website Tag Optimization</t>
+  </si>
+  <si>
+    <t>Google Tag Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimize the below :
+</t>
   </si>
 </sst>
 </file>
@@ -909,9 +919,6 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -925,16 +932,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -972,6 +970,18 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1268,137 +1278,137 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="48" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="48" style="2"/>
+    <col min="1" max="1" width="4.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="48" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="7">
+      <c r="B7" s="19">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="19"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="21"/>
     </row>
     <row r="11" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="5"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
+      <c r="B13" s="8"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="32.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.3">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1413,851 +1423,866 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="29.7265625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="30.08984375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="38.453125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="8.90625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.1796875" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="18"/>
+    <col min="1" max="1" width="4.36328125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="29.7265625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="30.08984375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="38.453125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="18">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="A7" s="18">
+      <c r="A7" s="14">
         <v>2</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="21"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J8" s="18" t="s">
+      <c r="H8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="21"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J9" s="18" t="s">
+      <c r="H9" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="21"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" s="18" t="s">
+      <c r="H10" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="21"/>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="14">
         <v>5</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="14">
         <v>10</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="21"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="18" t="s">
+      <c r="H12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="21"/>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="18" t="s">
+      <c r="H13" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="21"/>
+      <c r="B14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="21"/>
+      <c r="B15" s="17"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="18">
+      <c r="A16" s="14">
         <v>3</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="20" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="B17" s="21"/>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="B18" s="21"/>
-      <c r="C18" s="18" t="s">
+      <c r="H17" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B18" s="17"/>
+      <c r="C18" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="B19" s="21"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="21"/>
-      <c r="C20" s="18" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="21"/>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="14" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="21"/>
-      <c r="C22" s="18" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="72" x14ac:dyDescent="0.35">
-      <c r="B23" s="21"/>
-      <c r="C23" s="18" t="s">
+    <row r="23" spans="1:10" ht="48" x14ac:dyDescent="0.35">
+      <c r="B23" s="17"/>
+      <c r="C23" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="48" x14ac:dyDescent="0.35">
-      <c r="B24" s="21"/>
-      <c r="C24" s="18" t="s">
+    <row r="24" spans="1:10" ht="24" x14ac:dyDescent="0.35">
+      <c r="B24" s="17"/>
+      <c r="C24" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="48" x14ac:dyDescent="0.35">
+      <c r="B25" s="17"/>
+      <c r="C25" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D25" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F25" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G25" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J24" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="48" x14ac:dyDescent="0.35">
-      <c r="B25" s="21"/>
-      <c r="C25" s="18" t="s">
+      <c r="H25" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="48" x14ac:dyDescent="0.35">
+      <c r="B26" s="17"/>
+      <c r="C26" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E26" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F26" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G26" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H25" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="21"/>
-      <c r="C26" s="18" t="s">
+      <c r="H26" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+      <c r="B27" s="17"/>
+      <c r="C27" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D27" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E27" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F27" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G27" s="14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="21"/>
-    </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="18">
+      <c r="B28" s="17"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="14">
         <v>4</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="20" t="s">
+      <c r="B29" s="17"/>
+      <c r="C29" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B29" s="21"/>
-      <c r="C29" s="18" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B30" s="17"/>
+      <c r="C30" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="H29" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B30" s="21"/>
-      <c r="C30" s="18" t="s">
+      <c r="H30" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B31" s="17"/>
+      <c r="C31" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="H30" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B31" s="21"/>
-      <c r="C31" s="18" t="s">
+      <c r="H31" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B32" s="17"/>
+      <c r="C32" s="14" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B32" s="21"/>
-      <c r="C32" s="18" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B33" s="17"/>
+      <c r="C33" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="H32" s="18">
+      <c r="H33" s="14">
         <v>2</v>
       </c>
-      <c r="I32" s="18">
+      <c r="I33" s="14">
         <v>4</v>
       </c>
-      <c r="J32" s="18">
+      <c r="J33" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B33" s="21"/>
-      <c r="C33" s="18" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B34" s="17"/>
+      <c r="C34" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H34" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="I33" s="18">
+      <c r="I34" s="14">
         <v>2</v>
       </c>
-      <c r="J33" s="18">
+      <c r="J34" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="A35" s="18">
+    <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.35">
+      <c r="A36" s="14">
         <v>5</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B36" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C36" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B36" s="21"/>
-      <c r="C36" s="18" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B37" s="17"/>
+      <c r="C37" s="14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="B37" s="21"/>
-      <c r="C37" s="18" t="s">
+    <row r="38" spans="1:10" ht="24" x14ac:dyDescent="0.35">
+      <c r="B38" s="17"/>
+      <c r="C38" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D38" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="18" t="s">
+      <c r="F38" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="18">
+      <c r="H38" s="14">
         <v>2</v>
       </c>
-      <c r="I37" s="18">
+      <c r="I38" s="14">
         <v>4</v>
       </c>
-      <c r="J37" s="18">
+      <c r="J38" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B38" s="21"/>
-      <c r="C38" s="18" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B39" s="17"/>
+      <c r="C39" s="14" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B39" s="21"/>
-      <c r="C39" s="18" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B40" s="17"/>
+      <c r="C40" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B40" s="21"/>
-    </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B41" s="21"/>
+      <c r="B41" s="17"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B42" s="21"/>
+      <c r="B42" s="17"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="18">
+      <c r="B43" s="17"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="14">
         <v>6</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="20" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="B44" s="21"/>
-      <c r="C44" s="18" t="s">
+    <row r="45" spans="1:10" ht="24" x14ac:dyDescent="0.35">
+      <c r="B45" s="17"/>
+      <c r="C45" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D45" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H45" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="I44" s="18">
+      <c r="I45" s="14">
         <v>2</v>
       </c>
-      <c r="J44" s="18">
+      <c r="J45" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B45" s="21"/>
-      <c r="C45" s="18" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B46" s="17"/>
+      <c r="C46" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="H46" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="I45" s="18">
+      <c r="I46" s="14">
         <v>2</v>
       </c>
-      <c r="J45" s="18">
+      <c r="J46" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B46" s="21"/>
-      <c r="C46" s="18" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B47" s="17"/>
+      <c r="C47" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D47" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="I46" s="18">
+      <c r="I47" s="14">
         <v>2</v>
       </c>
-      <c r="J46" s="18">
+      <c r="J47" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B47" s="21"/>
-    </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B48" s="21"/>
+      <c r="B48" s="17"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B49" s="21"/>
+      <c r="B49" s="17"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B50" s="21"/>
+      <c r="B50" s="17"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A51" s="18">
+      <c r="B51" s="17"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" s="14">
         <v>7</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="20" t="s">
+      <c r="B52" s="17"/>
+      <c r="C52" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="24" x14ac:dyDescent="0.35">
-      <c r="B52" s="21"/>
-      <c r="C52" s="20" t="s">
+    <row r="53" spans="1:10" ht="24" x14ac:dyDescent="0.35">
+      <c r="B53" s="17"/>
+      <c r="C53" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D53" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H52" s="18">
+      <c r="H53" s="14">
         <v>2</v>
       </c>
-      <c r="I52" s="18">
+      <c r="I53" s="14">
         <v>4</v>
       </c>
-      <c r="J52" s="18">
+      <c r="J53" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="48" x14ac:dyDescent="0.35">
-      <c r="B53" s="21"/>
-      <c r="C53" s="20" t="s">
+    <row r="54" spans="1:10" ht="48" x14ac:dyDescent="0.35">
+      <c r="B54" s="17"/>
+      <c r="C54" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D54" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E54" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F53" s="18" t="s">
+      <c r="F54" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H53" s="18">
+      <c r="H54" s="14">
         <v>2</v>
       </c>
-      <c r="I53" s="18">
+      <c r="I54" s="14">
         <v>4</v>
       </c>
-      <c r="J53" s="18">
+      <c r="J54" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="48" x14ac:dyDescent="0.35">
-      <c r="B54" s="21"/>
-      <c r="C54" s="20" t="s">
+    <row r="55" spans="1:10" ht="48" x14ac:dyDescent="0.35">
+      <c r="B55" s="17"/>
+      <c r="C55" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="18" t="s">
+      <c r="D55" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E54" s="18" t="s">
+      <c r="E55" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F54" s="18" t="s">
+      <c r="F55" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H54" s="18">
+      <c r="H55" s="14">
         <v>7</v>
       </c>
-      <c r="I54" s="18">
+      <c r="I55" s="14">
         <v>15</v>
       </c>
-      <c r="J54" s="18">
+      <c r="J55" s="14">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="60" x14ac:dyDescent="0.35">
-      <c r="B55" s="21"/>
-      <c r="C55" s="20" t="s">
+    <row r="56" spans="1:10" ht="60" x14ac:dyDescent="0.35">
+      <c r="B56" s="17"/>
+      <c r="C56" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="D56" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E55" s="18" t="s">
+      <c r="E56" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F55" s="18" t="s">
+      <c r="F56" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H55" s="18">
+      <c r="H56" s="14">
         <v>2</v>
       </c>
-      <c r="I55" s="18">
+      <c r="I56" s="14">
         <v>4</v>
       </c>
-      <c r="J55" s="18">
+      <c r="J56" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B56" s="21"/>
-      <c r="C56" s="20" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B57" s="17"/>
+      <c r="C57" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F56" s="18" t="s">
+      <c r="F57" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H56" s="18">
+      <c r="H57" s="14">
         <v>7</v>
       </c>
-      <c r="I56" s="18">
+      <c r="I57" s="14">
         <v>15</v>
       </c>
-      <c r="J56" s="18">
+      <c r="J57" s="14">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B57" s="21"/>
-      <c r="C57" s="20" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B58" s="17"/>
+      <c r="C58" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F57" s="18" t="s">
+      <c r="F58" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="H57" s="18">
+      <c r="H58" s="14">
         <v>2</v>
       </c>
-      <c r="I57" s="18">
+      <c r="I58" s="14">
         <v>4</v>
       </c>
-      <c r="J57" s="18">
+      <c r="J58" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B58" s="21"/>
-      <c r="C58" s="20" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B59" s="17"/>
+      <c r="C59" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F58" s="18" t="s">
+      <c r="F59" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="H58" s="18">
+      <c r="H59" s="14">
         <v>2</v>
       </c>
-      <c r="I58" s="18">
+      <c r="I59" s="14">
         <v>4</v>
       </c>
-      <c r="J58" s="18">
+      <c r="J59" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B59" s="21"/>
-      <c r="C59" s="20" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B60" s="17"/>
+      <c r="C60" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F59" s="18" t="s">
+      <c r="F60" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="H59" s="18">
+      <c r="H60" s="14">
         <v>2</v>
       </c>
-      <c r="I59" s="18">
+      <c r="I60" s="14">
         <v>4</v>
       </c>
-      <c r="J59" s="18">
+      <c r="J60" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B60" s="21"/>
-      <c r="C60" s="20"/>
-    </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B61" s="21"/>
-      <c r="C61" s="20"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B62" s="21"/>
-      <c r="C62" s="20"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="16"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B63" s="21"/>
-      <c r="C63" s="20"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="16"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B64" s="21"/>
-      <c r="C64" s="20"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="16"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B65" s="21"/>
-      <c r="C65" s="20"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A67" s="18">
+      <c r="B65" s="17"/>
+      <c r="C65" s="16"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B66" s="17"/>
+      <c r="C66" s="16"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A68" s="14">
         <v>8</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B68" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C68" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C68" s="18" t="s">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C69" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="D69" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H68" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I68" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J68" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C69" s="18" t="s">
+      <c r="H69" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I69" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J69" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C70" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D69" s="18" t="s">
+      <c r="D70" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H69" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I69" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J69" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C70" s="18" t="s">
+      <c r="H70" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C71" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="D71" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H70" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I70" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J70" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A72" s="18">
+      <c r="H71" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A73" s="14">
         <v>9</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B73" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C73" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C73" s="18" t="s">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C74" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="H73" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I73" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J73" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C74" s="18" t="s">
+      <c r="H74" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I74" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J74" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C75" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H74" s="18" t="s">
+      <c r="H75" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="I74" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J74" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C75" s="18" t="s">
+      <c r="I75" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J75" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C76" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H75" s="18" t="s">
+      <c r="H76" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="I75" s="18" t="s">
+      <c r="I76" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="J75" s="18" t="s">
+      <c r="J76" s="14" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2266,8 +2291,8 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F25" r:id="rId1" xr:uid="{90063E75-569C-462E-B93A-6A610876D2FA}"/>
-    <hyperlink ref="F26" r:id="rId2" display="https://developers.google.com/search/docs/advanced/robots/create-robots-txt?visit_id=637598707007128202-2171794991&amp;rd=1" xr:uid="{98F5678B-2257-4823-A2A0-43B30F53D7B4}"/>
+    <hyperlink ref="F26" r:id="rId1" xr:uid="{90063E75-569C-462E-B93A-6A610876D2FA}"/>
+    <hyperlink ref="F27" r:id="rId2" display="https://developers.google.com/search/docs/advanced/robots/create-robots-txt?visit_id=637598707007128202-2171794991&amp;rd=1" xr:uid="{98F5678B-2257-4823-A2A0-43B30F53D7B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2284,26 +2309,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="13" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>